<commit_message>
Built-ins for __truediv__ and __floordiv__ were added
</commit_message>
<xml_diff>
--- a/Docs/Operators.xlsx
+++ b/Docs/Operators.xlsx
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,15 +137,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -154,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +167,17 @@
         <fgColor theme="7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -186,11 +188,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -200,12 +204,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="20% - Акцент3" xfId="5" builtinId="38"/>
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
     <cellStyle name="Акцент2" xfId="2" builtinId="33"/>
+    <cellStyle name="Акцент3" xfId="4" builtinId="37"/>
     <cellStyle name="Акцент4" xfId="3" builtinId="41"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -502,7 +508,7 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,13 +537,13 @@
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -548,13 +554,13 @@
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -565,13 +571,13 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1001,13 +1007,13 @@
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1039,13 +1045,13 @@
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1077,13 +1083,13 @@
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1153,13 +1159,13 @@
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G22" t="s">
@@ -1185,13 +1191,13 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1199,13 +1205,13 @@
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1227,13 +1233,13 @@
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1241,13 +1247,13 @@
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1255,13 +1261,13 @@
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1283,13 +1289,13 @@
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="B32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1297,13 +1303,13 @@
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1311,13 +1317,13 @@
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added built-ins for __mod__ and __pow__
</commit_message>
<xml_diff>
--- a/Docs/Operators.xlsx
+++ b/Docs/Operators.xlsx
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,16 +136,8 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,12 +164,6 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,27 +174,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="20% - Акцент3" xfId="5" builtinId="38"/>
+  <cellStyles count="5">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
     <cellStyle name="Акцент2" xfId="2" builtinId="33"/>
     <cellStyle name="Акцент3" xfId="4" builtinId="37"/>
@@ -508,7 +491,7 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,65 +512,65 @@
       <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="M4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="P5" s="2" t="s">
         <v>13</v>
       </c>
@@ -658,13 +641,13 @@
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -703,13 +686,13 @@
       <c r="S7" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="5">
         <v>1</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X7" t="s">
+      <c r="X7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -717,13 +700,13 @@
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -767,13 +750,13 @@
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -855,13 +838,13 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -893,13 +876,13 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -931,13 +914,13 @@
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1007,13 +990,13 @@
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1045,13 +1028,13 @@
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="B18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1083,13 +1066,13 @@
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="B19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1159,13 +1142,13 @@
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G22" t="s">
@@ -1191,13 +1174,13 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="B23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1205,13 +1188,13 @@
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1233,13 +1216,13 @@
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="B27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1247,13 +1230,13 @@
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="B28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1261,13 +1244,13 @@
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="B29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1289,13 +1272,13 @@
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="B32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1303,13 +1286,13 @@
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="B33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1317,13 +1300,13 @@
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="B34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>